<commit_message>
Corrected a few problems with hypolimnion fraction, and hypoxic fraction.
Script to deal with max depth units
</commit_message>
<xml_diff>
--- a/ohio2016/inputData/watershedAndMorphology/Lake_Volume_Final_101117_with_Extra_Acton_Visits.xlsx
+++ b/ohio2016/inputData/watershedAndMorphology/Lake_Volume_Final_101117_with_Extra_Acton_Visits.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JBEAULIE\GitRepository\mulitResSurvey\ohio2016\inputData\watershedAndMorphology\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9624"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-placeholder for now, need to update with correct values.</t>
+Values extrapolated from:
+L:\Priv\Cin\NRMRL\ReservoirEbullitionStudy\multiResSurvey2016\grtsDesign\acton\Bathymetry\ActonLake_Depth_SAreaVolume.txt</t>
         </r>
       </text>
     </comment>
@@ -152,7 +153,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-placeholder for now, need to update with correct values.</t>
+Values extrapolated from:
+L:\Priv\Cin\NRMRL\ReservoirEbullitionStudy\multiResSurvey2016\grtsDesign\acton\Bathymetry\ActonLake_Depth_SAreaVolume.txt</t>
         </r>
       </text>
     </comment>
@@ -200,7 +202,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-placeholder for now, need to update with correct values.</t>
+Values extrapolated from:
+L:\Priv\Cin\NRMRL\ReservoirEbullitionStudy\multiResSurvey2016\grtsDesign\acton\Bathymetry\ActonLake_Depth_SAreaVolume.txt</t>
         </r>
       </text>
     </comment>
@@ -224,7 +227,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-placeholder for now, need to update with correct values.</t>
+Values extrapolated from:
+L:\Priv\Cin\NRMRL\ReservoirEbullitionStudy\multiResSurvey2016\grtsDesign\acton\Bathymetry\ActonLake_Depth_SAreaVolume.txt</t>
         </r>
       </text>
     </comment>
@@ -272,31 +276,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-placeholder for now, need to update with correct values.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Beaulieu, Jake:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-placeholder for now, need to update with correct values.</t>
+Values extrapolated from:
+L:\Priv\Cin\NRMRL\ReservoirEbullitionStudy\multiResSurvey2016\grtsDesign\acton\Bathymetry\ActonLake_Depth_SAreaVolume.txt</t>
         </r>
       </text>
     </comment>
@@ -377,7 +358,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="77">
   <si>
     <t>Lake</t>
   </si>
@@ -666,13 +647,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -682,12 +662,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -781,10 +755,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1110,28 +1084,28 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="9" customWidth="1"/>
     <col min="5" max="5" width="16" style="9" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="9" customWidth="1"/>
     <col min="7" max="7" width="20" style="9" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="70.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="66.44140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="85.44140625" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="1"/>
+    <col min="8" max="8" width="20.42578125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="70.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="66.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="85.42578125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1146,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1214,7 +1188,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1227,14 +1201,14 @@
       <c r="D3" s="21">
         <v>6</v>
       </c>
-      <c r="E3" s="25">
-        <v>685212.36378500005</v>
+      <c r="E3" s="26">
+        <v>501326</v>
       </c>
       <c r="F3" s="21">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G3" s="26">
-        <v>4477110.9877699995</v>
+      <c r="G3" s="25">
+        <v>8083307.2224432984</v>
       </c>
       <c r="H3" s="13">
         <v>4.1553133731035201</v>
@@ -1254,7 +1228,7 @@
       </c>
       <c r="M3" s="24"/>
     </row>
-    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1267,14 +1241,14 @@
       <c r="D4" s="21">
         <v>5</v>
       </c>
-      <c r="E4" s="25">
-        <v>685212.36378500005</v>
+      <c r="E4" s="26">
+        <v>1169765.86971222</v>
       </c>
       <c r="F4" s="21">
         <v>6.5</v>
       </c>
-      <c r="G4" s="26">
-        <v>4477110.9877699995</v>
+      <c r="G4" s="25">
+        <v>326433.16704165447</v>
       </c>
       <c r="H4" s="13">
         <v>4.1553133731035201</v>
@@ -1294,7 +1268,7 @@
       </c>
       <c r="M4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1307,14 +1281,14 @@
       <c r="D5" s="21">
         <v>6</v>
       </c>
-      <c r="E5" s="25">
-        <v>685212.36378500005</v>
+      <c r="E5" s="26">
+        <v>501326</v>
       </c>
       <c r="F5" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="26">
-        <v>4477110.9877699995</v>
+      <c r="G5" s="25">
+        <v>0</v>
       </c>
       <c r="H5" s="13">
         <v>4.1553133731035201</v>
@@ -1334,7 +1308,7 @@
       </c>
       <c r="M5" s="24"/>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
@@ -1347,8 +1321,8 @@
       <c r="D6" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>38</v>
+      <c r="E6" s="22">
+        <v>0</v>
       </c>
       <c r="F6" s="22">
         <v>5.2745639999999998</v>
@@ -1374,7 +1348,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1387,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1427,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1492,7 +1466,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>5</v>
       </c>
@@ -1511,8 +1485,8 @@
       <c r="F10" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>38</v>
+      <c r="G10" s="20">
+        <v>0</v>
       </c>
       <c r="H10" s="17">
         <v>17.210276009354899</v>
@@ -1534,7 +1508,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1547,8 +1521,8 @@
       <c r="D11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>38</v>
+      <c r="E11" s="10">
+        <v>0</v>
       </c>
       <c r="F11" s="21">
         <v>3.5</v>
@@ -1573,7 +1547,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>7</v>
       </c>
@@ -1615,7 +1589,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1628,8 +1602,8 @@
       <c r="D13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>38</v>
+      <c r="E13" s="10">
+        <v>0</v>
       </c>
       <c r="F13" s="21">
         <v>8.5</v>
@@ -1657,7 +1631,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>8</v>
       </c>
@@ -1699,7 +1673,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1712,14 +1686,14 @@
       <c r="D15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>38</v>
+      <c r="E15" s="10">
+        <v>0</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>38</v>
+      <c r="G15" s="10">
+        <v>0</v>
       </c>
       <c r="H15" s="13">
         <v>1.3522106568524499</v>
@@ -1738,7 +1712,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>10</v>
       </c>
@@ -1778,7 +1752,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1791,14 +1765,14 @@
       <c r="D17" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>38</v>
+      <c r="E17" s="10">
+        <v>0</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>38</v>
+      <c r="G17" s="10">
+        <v>0</v>
       </c>
       <c r="H17" s="13">
         <v>2.84508720574452</v>
@@ -1817,7 +1791,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
@@ -1830,14 +1804,14 @@
       <c r="D18" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>38</v>
+      <c r="E18" s="22">
+        <v>0</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="20" t="s">
-        <v>38</v>
+      <c r="G18" s="20">
+        <v>0</v>
       </c>
       <c r="H18" s="17">
         <v>2.7612303555269699</v>
@@ -1857,7 +1831,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1899,7 +1873,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>14</v>
       </c>
@@ -1912,8 +1886,8 @@
       <c r="D20" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="22" t="s">
-        <v>38</v>
+      <c r="E20" s="22">
+        <v>0</v>
       </c>
       <c r="F20" s="22">
         <v>0.53461919999999996</v>
@@ -1939,7 +1913,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1978,7 +1952,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
@@ -2018,7 +1992,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -2031,14 +2005,14 @@
       <c r="D23" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>38</v>
+      <c r="E23" s="10">
+        <v>0</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>38</v>
+      <c r="G23" s="10">
+        <v>0</v>
       </c>
       <c r="H23" s="13">
         <v>0.94049311518134504</v>
@@ -2060,7 +2034,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>18</v>
       </c>
@@ -2100,7 +2074,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2142,7 +2116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>24</v>
       </c>
@@ -2182,7 +2156,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -2224,7 +2198,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>20</v>
       </c>
@@ -2266,7 +2240,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -2285,8 +2259,8 @@
       <c r="F29" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>38</v>
+      <c r="G29" s="10">
+        <v>0</v>
       </c>
       <c r="H29" s="13">
         <v>4.2087309424934602</v>
@@ -2305,7 +2279,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>22</v>
       </c>
@@ -2319,13 +2293,13 @@
         <v>38</v>
       </c>
       <c r="E30" s="22">
-        <v>8014619.9365929998</v>
+        <v>0</v>
       </c>
       <c r="F30" s="22">
         <v>4.5</v>
       </c>
-      <c r="G30" s="20" t="s">
-        <v>38</v>
+      <c r="G30" s="22">
+        <v>8014619.9365929998</v>
       </c>
       <c r="H30" s="17">
         <v>4.1391400313691289</v>
@@ -2345,7 +2319,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -2384,7 +2358,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>25</v>
       </c>
@@ -2424,7 +2398,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
@@ -2443,8 +2417,8 @@
       <c r="F33" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G33" s="10" t="s">
-        <v>38</v>
+      <c r="G33" s="10">
+        <v>0</v>
       </c>
       <c r="H33" s="13">
         <v>3.62598683127041</v>
@@ -2463,7 +2437,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>27</v>
       </c>
@@ -2503,7 +2477,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -2545,7 +2519,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>29</v>
       </c>
@@ -2558,14 +2532,14 @@
       <c r="D36" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="22" t="s">
-        <v>38</v>
+      <c r="E36" s="22">
+        <v>0</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="G36" s="20" t="s">
-        <v>38</v>
+      <c r="G36" s="20">
+        <v>0</v>
       </c>
       <c r="H36" s="17">
         <v>1.9395218563602099</v>
@@ -2585,19 +2559,19 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
       <c r="J39" s="9"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I40" s="2"/>
       <c r="J40" s="9"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="3"/>
       <c r="C41" s="1"/>
@@ -2611,7 +2585,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="3"/>
       <c r="C42" s="1"/>

</xml_diff>